<commit_message>
added serial and initial data of virtual account book
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-fm/src/main/resources/plugin/fm/oob/data/fm.number.xlsx
+++ b/vertx-pin/zero-fm/src/main/resources/plugin/fm/oob/data/fm.number.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/ox-workshop/vertx-zero/vertx-pin/zero-fm/src/main/resources/plugin/fm/oob/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evgreen\Downloads\vie\code\vertx-zero\vertx-pin\zero-fm\src\main\resources\plugin\fm\oob\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BA5470-2FEA-B745-9257-4204531CA619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B651326-3C0C-4490-8F68-D6DD0C8D6A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68340" yWindow="-5880" windowWidth="46400" windowHeight="27220" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-APP" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
   <si>
     <t>code</t>
   </si>
@@ -233,6 +233,22 @@
   </si>
   <si>
     <t>NUM.SETTLEMENT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f2b8c448-976c-4b11-a30b-95600db19658</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哑房账本编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ABV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NUM.ACCOUNT.BOOK.VIRTUAL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -240,7 +256,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -720,39 +736,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71967B7B-87F9-4846-9FA6-1A2C9E90AB57}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="54.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.625" style="7" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.5" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="2"/>
+    <col min="17" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="M1" s="1"/>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -776,7 +792,7 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>17</v>
       </c>
@@ -820,7 +836,7 @@
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -864,7 +880,7 @@
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>12</v>
       </c>
@@ -899,7 +915,7 @@
       <c r="L5" s="15"/>
       <c r="M5" s="14"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>6</v>
       </c>
@@ -934,31 +950,31 @@
       <c r="L6" s="15"/>
       <c r="M6" s="14"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J7" s="5">
         <v>1</v>
@@ -966,31 +982,27 @@
       <c r="K7" s="14" t="b">
         <v>0</v>
       </c>
-      <c r="L7" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="14" t="b">
-        <v>1</v>
-      </c>
+      <c r="L7" s="15"/>
+      <c r="M7" s="14"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>42</v>
@@ -1012,24 +1024,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>42</v>
@@ -1051,15 +1063,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>57</v>
@@ -1068,7 +1080,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>42</v>
@@ -1087,6 +1099,45 @@
         <v>43</v>
       </c>
       <c r="M10" s="14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5">
+        <v>4</v>
+      </c>
+      <c r="J11" s="5">
+        <v>1</v>
+      </c>
+      <c r="K11" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="14" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1096,5 +1147,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>